<commit_message>
Added columns for actual impostor speaker in results
</commit_message>
<xml_diff>
--- a/test_results/00_04_050.xlsx
+++ b/test_results/00_04_050.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="78">
   <si>
     <t>LIVING_ROOM</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>-30 - ALEX</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>Yes</t>
@@ -262,7 +259,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -277,6 +274,12 @@
     </font>
     <font/>
     <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -512,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -529,7 +532,7 @@
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -562,14 +565,20 @@
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="3" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -586,7 +595,7 @@
     <xf borderId="9" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -607,7 +616,7 @@
     <xf borderId="12" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -981,7 +990,7 @@
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="17" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -994,7 +1003,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -1002,56 +1011,56 @@
         <v>7</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="19" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="12">
         <v>1.0</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>24</v>
+      <c r="E11" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="F11" s="14"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -1066,7 +1075,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>5</v>
@@ -1081,11 +1090,11 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="17" t="s">
-        <v>27</v>
       </c>
       <c r="F14" s="7">
         <v>0.0</v>
@@ -1096,8 +1105,8 @@
         <v>10</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="17" t="s">
-        <v>28</v>
+      <c r="C15" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="10" t="s">
@@ -1109,15 +1118,15 @@
       <c r="A16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="21">
         <v>0.0</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="20"/>
+      <c r="C16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="22"/>
       <c r="E16" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="4"/>
     </row>
@@ -2157,7 +2166,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
@@ -2176,7 +2185,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
@@ -2190,28 +2199,28 @@
         <v>8</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="21" t="s">
-        <v>30</v>
+      <c r="C4" s="23" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="16">
         <v>0.0</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>31</v>
+      <c r="C5" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="19" t="s">
-        <v>24</v>
+      <c r="E5" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="F5" s="16">
         <v>0.0</v>
@@ -2219,7 +2228,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
@@ -2227,24 +2236,24 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="25" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -2253,31 +2262,31 @@
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="24" t="s">
-        <v>27</v>
+      <c r="E8" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="F8" s="7">
         <v>0.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="19" t="s">
-        <v>24</v>
+      <c r="E9" s="20" t="s">
+        <v>23</v>
       </c>
       <c r="F9" s="14"/>
     </row>
@@ -2316,36 +2325,36 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="17" t="s">
-        <v>27</v>
+      <c r="E12" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="F12" s="7">
         <v>0.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
-        <v>20</v>
+      <c r="A13" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="B13" s="16">
         <v>1.0</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>31</v>
+      <c r="C13" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="16">
         <v>1.0</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>32</v>
+      <c r="E13" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -3415,31 +3424,31 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="7">
         <v>0.0</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>27</v>
+      <c r="C4" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="D4" s="7">
         <v>0.0</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="7">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="s">
-        <v>35</v>
+      <c r="A5" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="6" t="s">
@@ -3448,12 +3457,12 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="25" t="s">
-        <v>20</v>
+      <c r="A6" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="8" t="s">
@@ -3462,26 +3471,26 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="19" t="s">
-        <v>23</v>
+      <c r="A7" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="14"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
@@ -3496,7 +3505,7 @@
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -3510,30 +3519,30 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="7">
         <v>0.0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="7">
         <v>0.0</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="9" t="s">
@@ -3547,25 +3556,25 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="17" t="s">
-        <v>39</v>
+      <c r="E12" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="26" t="s">
-        <v>24</v>
+      <c r="C13" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="14"/>
-      <c r="E13" s="18" t="s">
-        <v>31</v>
+      <c r="E13" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="F13" s="16">
         <v>1.0</v>
@@ -3581,12 +3590,12 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3607,61 +3616,61 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="7">
         <v>0.0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="29" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="27" t="s">
-        <v>44</v>
       </c>
       <c r="D17" s="7">
         <v>0.0</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="17" t="s">
-        <v>46</v>
+      <c r="C18" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="28" t="s">
-        <v>47</v>
+      <c r="A19" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="18" t="s">
-        <v>24</v>
+      <c r="C19" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="17" t="s">
-        <v>22</v>
+      <c r="E19" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="F19" s="7">
         <v>0.0</v>
@@ -4685,248 +4694,248 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="G1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="29" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="30" t="s">
+      <c r="C2" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B3" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="D3" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="30" t="s">
+      <c r="F3" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B4" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C6" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="42">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="33" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="31" t="s">
+      <c r="C13" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="40">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>